<commit_message>
Renamed metro_budget to metro_budget_worked so I could have allversions in folder
</commit_message>
<xml_diff>
--- a/metro_budget.xlsx
+++ b/metro_budget.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26019"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\metro_budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary van Valkenburg\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123DBE1D-ED06-4FD2-8244-EB4886B03004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{BAAD70D2-3286-47C7-9C4C-6DF3580ADD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADAF992F-2F25-409B-818D-4B9B36D48F80}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="90" windowWidth="21877" windowHeight="13080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="AllDepartments">metro_budget!$A$1:$A$52</definedName>
-    <definedName name="dataset">metro_budget!$A$1:$K$52</definedName>
-    <definedName name="Departments">metro_budget!$A$56:$A$61</definedName>
-    <definedName name="Headers">metro_budget!$A$1:$K$1</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,30 +33,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Department</t>
   </si>
@@ -275,16 +247,13 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
-  </si>
-  <si>
-    <t>Avg_diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,7 +397,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -843,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -883,7 +852,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -989,7 +958,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1131,7 +1100,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1139,28 +1108,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1191,11 +1158,8 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1226,12 +1190,8 @@
       <c r="J2">
         <v>-21269107.77</v>
       </c>
-      <c r="K2">
-        <f>AVERAGE(D2,G2,J2)</f>
-        <v>-24336639.273333233</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1262,12 +1222,8 @@
       <c r="J3">
         <v>-436.96000000001999</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K52" si="0">AVERAGE(D3,G3,J3)</f>
-        <v>-10129.553333333331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1298,12 +1254,8 @@
       <c r="J4">
         <v>-97416.950000001103</v>
       </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>-58488.72666666747</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1334,12 +1286,8 @@
       <c r="J5">
         <v>-262277.08999999898</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>-644371.69999999867</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1370,12 +1318,8 @@
       <c r="J6">
         <v>-85.710000000079106</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>-8072.8499999999885</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1406,12 +1350,8 @@
       <c r="J7">
         <v>-398759.91999999899</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>-373701.76666666596</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1442,12 +1382,8 @@
       <c r="J8">
         <v>-241564.68</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>-228278.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1478,12 +1414,8 @@
       <c r="J9">
         <v>-796900.47000000405</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>-779371.89000000141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1514,12 +1446,8 @@
       <c r="J10">
         <v>-9181.0800000000108</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>-24227.623333333275</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1550,12 +1478,8 @@
       <c r="J11">
         <v>-311228.08999999898</v>
       </c>
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>-103742.69666666632</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1586,12 +1510,8 @@
       <c r="J12">
         <v>-306086.86</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>-338411.97666666534</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1622,12 +1542,8 @@
       <c r="J13">
         <v>-150323.329999999</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>-180152.35333333295</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1658,12 +1574,8 @@
       <c r="J14">
         <v>-21210.119999999901</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>-11429.923333333229</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1694,12 +1606,8 @@
       <c r="J15">
         <v>-4502589.1500000302</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>-4069060.0000000186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1730,12 +1638,8 @@
       <c r="J16">
         <v>-106.999999999068</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>-26787.486666666631</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1766,12 +1670,8 @@
       <c r="J17">
         <v>-965742.96</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>-683843.13333333295</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1802,12 +1702,8 @@
       <c r="J18">
         <v>-374962.91</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>-237871.02333333297</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1838,12 +1734,8 @@
       <c r="J19">
         <v>-576344.08999999403</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>-558091.21666666702</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1874,12 +1766,8 @@
       <c r="J20">
         <v>-116.46000003814601</v>
       </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>-3810.6433333406817</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1910,12 +1798,8 @@
       <c r="J21">
         <v>-888926.91000000294</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>-1551281.9100000076</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1946,12 +1830,8 @@
       <c r="J22">
         <v>-745.22999999672095</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>-114375.79333333323</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1982,12 +1862,8 @@
       <c r="J23">
         <v>-601242.55999998702</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>-796290.97666667739</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2018,12 +1894,8 @@
       <c r="J24">
         <v>-72.879999999888199</v>
       </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>-19263.089999999829</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2054,12 +1926,8 @@
       <c r="J25">
         <v>-1724.8999999999601</v>
       </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>-4893.7199999999666</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2090,12 +1958,8 @@
       <c r="J26">
         <v>-313464.78999999998</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>-360391.89333333302</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2126,12 +1990,8 @@
       <c r="J27">
         <v>0</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2162,12 +2022,8 @@
       <c r="J28">
         <v>-132614.93999999901</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>-176479.22999999937</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2198,12 +2054,8 @@
       <c r="J29">
         <v>-35.329999999143098</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>-50728.72666666608</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2234,12 +2086,8 @@
       <c r="J30">
         <v>-35290.389999991203</v>
       </c>
-      <c r="K30">
-        <f t="shared" si="0"/>
-        <v>-62460.669999994228</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2270,12 +2118,8 @@
       <c r="J31">
         <v>-69308.659999999596</v>
       </c>
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>-51568.039999999601</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2306,12 +2150,8 @@
       <c r="J32">
         <v>-169827.98</v>
       </c>
-      <c r="K32">
-        <f t="shared" si="0"/>
-        <v>-118034.93000000005</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2342,12 +2182,8 @@
       <c r="J33">
         <v>-5456610.5900001498</v>
       </c>
-      <c r="K33">
-        <f t="shared" si="0"/>
-        <v>-5159310.7933333265</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2378,12 +2214,8 @@
       <c r="J34">
         <v>-115798.49</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>-136050.49999999962</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2414,12 +2246,8 @@
       <c r="J35">
         <v>0</v>
       </c>
-      <c r="K35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -2450,12 +2278,8 @@
       <c r="J36">
         <v>-101084.71</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>-107198.16000000008</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -2486,12 +2310,8 @@
       <c r="J37">
         <v>-188181.66</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="0"/>
-        <v>-126930.23666666658</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -2522,12 +2342,8 @@
       <c r="J38">
         <v>-136.73999999987399</v>
       </c>
-      <c r="K38">
-        <f t="shared" si="0"/>
-        <v>-18704.986666666489</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -2558,12 +2374,8 @@
       <c r="J39">
         <v>-79036.130000000296</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="0"/>
-        <v>-109994.99333333345</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -2594,12 +2406,8 @@
       <c r="J40">
         <v>-610436.29000002099</v>
       </c>
-      <c r="K40">
-        <f t="shared" si="0"/>
-        <v>-1098951.4133333552</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -2630,12 +2438,8 @@
       <c r="J41">
         <v>-82077.349999997707</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="0"/>
-        <v>-133257.82333333293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2666,12 +2470,8 @@
       <c r="J42">
         <v>-36.250000059604602</v>
       </c>
-      <c r="K42">
-        <f t="shared" si="0"/>
-        <v>-805642.42000006372</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -2702,12 +2502,8 @@
       <c r="J43">
         <v>-346517.43</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="0"/>
-        <v>-300866.52666666568</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -2738,12 +2534,8 @@
       <c r="J44">
         <v>-58.749999988824101</v>
       </c>
-      <c r="K44">
-        <f t="shared" si="0"/>
-        <v>-180380.9633333206</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -2774,12 +2566,8 @@
       <c r="J45">
         <v>-640550.34000001801</v>
       </c>
-      <c r="K45">
-        <f t="shared" si="0"/>
-        <v>-1183270.7766666792</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -2810,12 +2598,8 @@
       <c r="J46">
         <v>-12346.84</v>
       </c>
-      <c r="K46">
-        <f t="shared" si="0"/>
-        <v>-7240.50000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2846,12 +2630,8 @@
       <c r="J47">
         <v>-21970.8200000822</v>
       </c>
-      <c r="K47">
-        <f t="shared" si="0"/>
-        <v>-19567.480000009065</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -2882,12 +2662,8 @@
       <c r="J48">
         <v>-407449.76000000199</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="0"/>
-        <v>-303274.87666666665</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -2918,12 +2694,8 @@
       <c r="J49">
         <v>0</v>
       </c>
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>-2944.563333333323</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2954,12 +2726,8 @@
       <c r="J50">
         <v>0</v>
       </c>
-      <c r="K50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2990,12 +2758,8 @@
       <c r="J51">
         <v>-98056.689999999406</v>
       </c>
-      <c r="K51">
-        <f t="shared" si="0"/>
-        <v>-178190.57666666713</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3026,12 +2790,8 @@
       <c r="J52">
         <v>-264764.74</v>
       </c>
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>-232369.01999999932</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -3045,118 +2805,34 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>18</v>
       </c>
-      <c r="B56">
-        <f>INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>-36209.629999999903</v>
-      </c>
-      <c r="C56">
-        <f>INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>-27292.159999999902</v>
-      </c>
-      <c r="D56">
-        <f>INDEX(dataset,MATCH($A56,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-9181.0800000000108</v>
-      </c>
-      <c r="E56">
-        <f>MATCH(A56,AllDepartments,0)</f>
-        <v>10</v>
-      </c>
-      <c r="F56">
-        <f>MATCH(B55,Headers,0)</f>
-        <v>4</v>
-      </c>
-      <c r="G56" cm="1">
-        <f t="array" ref="G56">INDEX(dataset,E56,F56)</f>
-        <v>-36209.629999999903</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>19</v>
       </c>
-      <c r="B57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>0</v>
-      </c>
-      <c r="C57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <f>INDEX(dataset,MATCH($A57,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-311228.08999999898</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>26</v>
       </c>
-      <c r="B58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>-149396.1</v>
-      </c>
-      <c r="C58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>-189254.05999999901</v>
-      </c>
-      <c r="D58">
-        <f>INDEX(dataset,MATCH($A58,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-374962.91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>32</v>
       </c>
-      <c r="B59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>-12230.809999999799</v>
-      </c>
-      <c r="C59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>-45485.579999999798</v>
-      </c>
-      <c r="D59">
-        <f>INDEX(dataset,MATCH($A59,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-72.879999999888199</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>33</v>
       </c>
-      <c r="B60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>-4950.4699999999102</v>
-      </c>
-      <c r="C60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>-8005.79000000003</v>
-      </c>
-      <c r="D60">
-        <f>INDEX(dataset,MATCH($A60,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-1724.8999999999601</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>49</v>
-      </c>
-      <c r="B61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(B$55,Headers,0))</f>
-        <v>-184239.79</v>
-      </c>
-      <c r="C61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(C$55,Headers,0))</f>
-        <v>-133456.33000000101</v>
-      </c>
-      <c r="D61">
-        <f>INDEX(dataset,MATCH($A61,AllDepartments,0), MATCH(D$55,Headers,0))</f>
-        <v>-82077.349999997707</v>
       </c>
     </row>
   </sheetData>
@@ -3168,17 +2844,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB99AC6-F6B8-4A26-96BE-D02EE21B4B6C}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3186,7 +2862,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3194,7 +2870,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3202,7 +2878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -3210,7 +2886,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3218,7 +2894,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -3226,7 +2902,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -3234,7 +2910,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3242,7 +2918,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -3250,7 +2926,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>